<commit_message>
Correct typos in the model parameter csv
Former-commit-id: bdcfcc0025b0e9cf0a65983860b73a1d22dd416e [formerly 36fdf1ca0dd1e1a6f4c4bcffb8def541d62dab5d]
Former-commit-id: 350363eb87fd80e2e8b8a0181394a6a262c89a1a
Former-commit-id: 9411c690953e45ef039b690a34ba59714dede8ab
Former-commit-id: 4c02582e76c004ab009d4658ba2a015de71d7aea
</commit_message>
<xml_diff>
--- a/etc/Model-based-algorithms-best-parameteres.xlsx
+++ b/etc/Model-based-algorithms-best-parameteres.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ideal_parameters_low_noise" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -571,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,10 +914,7 @@
       </c>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="AB3" s="3" t="str">
-        <f t="shared" ref="AB3" si="0">"DS"&amp;COLUMN(AB3)-1</f>
-        <v>DS27</v>
-      </c>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -929,14 +926,10 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="AB5" s="4">
-        <v>0.2</v>
-      </c>
+      <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="AB6" s="4">
-        <v>5.5E-2</v>
-      </c>
+      <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="AB7" s="3"/>
@@ -952,95 +945,96 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f>"DS0"&amp;COLUMN(F8)-1</f>
+        <f>"DS0"&amp;COLUMN(F8)-2</f>
+        <v>DS04</v>
+      </c>
+      <c r="G8" s="3" t="str">
+        <f t="shared" ref="G8:AB8" si="0">"DS0"&amp;COLUMN(G8)-2</f>
         <v>DS05</v>
       </c>
-      <c r="G8" s="3" t="str">
-        <f t="shared" ref="G8:M8" si="1">"DS0"&amp;COLUMN(G8)-1</f>
+      <c r="H8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS06</v>
       </c>
-      <c r="H8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS07</v>
       </c>
-      <c r="I8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="J8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS08</v>
       </c>
-      <c r="J8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="K8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS09</v>
       </c>
-      <c r="K8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="L8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS010</v>
       </c>
-      <c r="L8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="M8" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>DS011</v>
       </c>
-      <c r="M8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(M8)-1</f>
-        <v>DS12</v>
-      </c>
       <c r="N8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(N8)-1</f>
-        <v>DS13</v>
+        <f t="shared" si="0"/>
+        <v>DS012</v>
       </c>
       <c r="O8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(O8)-1</f>
-        <v>DS14</v>
+        <f t="shared" si="0"/>
+        <v>DS013</v>
       </c>
       <c r="P8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(P8)-1</f>
-        <v>DS15</v>
+        <f t="shared" si="0"/>
+        <v>DS014</v>
       </c>
       <c r="Q8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Q8)-1</f>
-        <v>DS16</v>
+        <f t="shared" si="0"/>
+        <v>DS015</v>
       </c>
       <c r="R8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(R8)-1</f>
-        <v>DS17</v>
+        <f t="shared" si="0"/>
+        <v>DS016</v>
       </c>
       <c r="S8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(S8)-1</f>
-        <v>DS18</v>
+        <f t="shared" si="0"/>
+        <v>DS017</v>
       </c>
       <c r="T8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(T8)-1</f>
-        <v>DS19</v>
+        <f t="shared" si="0"/>
+        <v>DS018</v>
       </c>
       <c r="U8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(U8)-1</f>
-        <v>DS20</v>
+        <f t="shared" si="0"/>
+        <v>DS019</v>
       </c>
       <c r="V8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(V8)-1</f>
-        <v>DS21</v>
+        <f t="shared" si="0"/>
+        <v>DS020</v>
       </c>
       <c r="W8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(W8)-1</f>
-        <v>DS22</v>
+        <f t="shared" si="0"/>
+        <v>DS021</v>
       </c>
       <c r="X8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(X8)-1</f>
-        <v>DS23</v>
+        <f t="shared" si="0"/>
+        <v>DS022</v>
       </c>
       <c r="Y8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Y8)-1</f>
-        <v>DS24</v>
+        <f t="shared" si="0"/>
+        <v>DS023</v>
       </c>
       <c r="Z8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Z8)-1</f>
-        <v>DS25</v>
+        <f t="shared" si="0"/>
+        <v>DS024</v>
       </c>
       <c r="AA8" s="3" t="str">
-        <f>"DS"&amp;COLUMN(AA8)-1</f>
-        <v>DS26</v>
-      </c>
-      <c r="AB8" s="4">
-        <v>1.125</v>
+        <f t="shared" si="0"/>
+        <v>DS025</v>
+      </c>
+      <c r="AB8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DS026</v>
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
@@ -1069,9 +1063,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="4">
-        <v>9.375</v>
-      </c>
+      <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -1152,7 +1144,9 @@
       <c r="AA10" s="4">
         <v>0.2</v>
       </c>
-      <c r="AB10" s="4"/>
+      <c r="AB10" s="4">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
@@ -1232,7 +1226,7 @@
         <v>2.8823999999999999E-2</v>
       </c>
       <c r="AB11" s="4">
-        <v>0.02</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
@@ -1344,7 +1338,7 @@
         <v>1.8529</v>
       </c>
       <c r="AB13" s="4">
-        <v>0.25</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
@@ -1425,7 +1419,7 @@
         <v>8.8234999999999992</v>
       </c>
       <c r="AB14" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
@@ -1455,7 +1449,7 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
-      <c r="AB15" s="3"/>
+      <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1537,7 +1531,7 @@
         <v>6.9412000000000001E-2</v>
       </c>
       <c r="AB16" s="4">
-        <v>3.7125000000000001E-3</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
@@ -1567,9 +1561,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="4">
-        <v>0.4</v>
-      </c>
+      <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -1650,7 +1642,9 @@
       <c r="AA18" s="4">
         <v>0.25</v>
       </c>
-      <c r="AB18" s="3"/>
+      <c r="AB18" s="4">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
@@ -1729,7 +1723,9 @@
       <c r="AA19" s="4">
         <v>2.9412000000000001E-2</v>
       </c>
-      <c r="AB19" s="3"/>
+      <c r="AB19" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
@@ -1758,10 +1754,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
-      <c r="AB20" s="3" t="str">
-        <f t="shared" ref="AB20" si="2">"DS"&amp;COLUMN(AB20)-1</f>
-        <v>DS27</v>
-      </c>
+      <c r="AB20" s="3"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -1842,7 +1835,9 @@
       <c r="AA21" s="4">
         <v>3.3E-3</v>
       </c>
-      <c r="AB21" s="3"/>
+      <c r="AB21" s="4">
+        <v>3.7125000000000001E-3</v>
+      </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -1922,7 +1917,7 @@
         <v>0.56471000000000005</v>
       </c>
       <c r="AB22" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
@@ -1952,9 +1947,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
@@ -1983,7 +1976,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="4"/>
+      <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
@@ -1997,95 +1990,96 @@
         <v>12</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>"DS0"&amp;COLUMN(F25)-1</f>
+        <f t="shared" ref="F25:AA25" si="1">"DS0"&amp;COLUMN(F25)-2</f>
+        <v>DS04</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS05</v>
       </c>
-      <c r="G25" s="3" t="str">
-        <f t="shared" ref="G25:M25" si="3">"DS0"&amp;COLUMN(G25)-1</f>
+      <c r="H25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS06</v>
       </c>
-      <c r="H25" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS07</v>
       </c>
-      <c r="I25" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="J25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS08</v>
       </c>
-      <c r="J25" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="K25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS09</v>
       </c>
-      <c r="K25" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="L25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS010</v>
       </c>
-      <c r="L25" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="M25" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>DS011</v>
       </c>
-      <c r="M25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(M25)-1</f>
-        <v>DS12</v>
-      </c>
       <c r="N25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(N25)-1</f>
-        <v>DS13</v>
+        <f t="shared" si="1"/>
+        <v>DS012</v>
       </c>
       <c r="O25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(O25)-1</f>
-        <v>DS14</v>
+        <f t="shared" si="1"/>
+        <v>DS013</v>
       </c>
       <c r="P25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(P25)-1</f>
-        <v>DS15</v>
+        <f t="shared" si="1"/>
+        <v>DS014</v>
       </c>
       <c r="Q25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Q25)-1</f>
-        <v>DS16</v>
+        <f t="shared" si="1"/>
+        <v>DS015</v>
       </c>
       <c r="R25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(R25)-1</f>
-        <v>DS17</v>
+        <f t="shared" si="1"/>
+        <v>DS016</v>
       </c>
       <c r="S25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(S25)-1</f>
-        <v>DS18</v>
+        <f t="shared" si="1"/>
+        <v>DS017</v>
       </c>
       <c r="T25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(T25)-1</f>
-        <v>DS19</v>
+        <f t="shared" si="1"/>
+        <v>DS018</v>
       </c>
       <c r="U25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(U25)-1</f>
-        <v>DS20</v>
+        <f t="shared" si="1"/>
+        <v>DS019</v>
       </c>
       <c r="V25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(V25)-1</f>
-        <v>DS21</v>
+        <f t="shared" si="1"/>
+        <v>DS020</v>
       </c>
       <c r="W25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(W25)-1</f>
-        <v>DS22</v>
+        <f t="shared" si="1"/>
+        <v>DS021</v>
       </c>
       <c r="X25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(X25)-1</f>
-        <v>DS23</v>
+        <f t="shared" si="1"/>
+        <v>DS022</v>
       </c>
       <c r="Y25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Y25)-1</f>
-        <v>DS24</v>
+        <f t="shared" si="1"/>
+        <v>DS023</v>
       </c>
       <c r="Z25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(Z25)-1</f>
-        <v>DS25</v>
+        <f t="shared" si="1"/>
+        <v>DS024</v>
       </c>
       <c r="AA25" s="3" t="str">
-        <f>"DS"&amp;COLUMN(AA25)-1</f>
-        <v>DS26</v>
-      </c>
-      <c r="AB25" s="4">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>DS025</v>
+      </c>
+      <c r="AB25" s="3" t="str">
+        <f t="shared" ref="AB25" si="2">"DS"&amp;COLUMN(AB25)-1</f>
+        <v>DS27</v>
       </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
@@ -2115,9 +2109,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
-      <c r="AB26" s="4">
-        <v>10</v>
-      </c>
+      <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -2198,7 +2190,9 @@
       <c r="AA27" s="4">
         <v>0.35881999999999997</v>
       </c>
-      <c r="AB27" s="4"/>
+      <c r="AB27" s="4">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -2278,7 +2272,7 @@
         <v>3.1175999999999999E-2</v>
       </c>
       <c r="AB28" s="4">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
@@ -2390,7 +2384,7 @@
         <v>1.5882000000000001</v>
       </c>
       <c r="AB30" s="4">
-        <v>0.5625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
@@ -2471,7 +2465,7 @@
         <v>9.4117999999999995</v>
       </c>
       <c r="AB31" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
@@ -2583,7 +2577,7 @@
         <v>5.5294000000000003E-2</v>
       </c>
       <c r="AB33" s="4">
-        <v>9.5499999999999995E-3</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.25">
@@ -2613,9 +2607,7 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
-      <c r="AB34" s="4">
-        <v>0.1</v>
-      </c>
+      <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -2695,6 +2687,9 @@
       </c>
       <c r="AA35" s="4">
         <v>0.63234999999999997</v>
+      </c>
+      <c r="AB35" s="4">
+        <v>0.5625</v>
       </c>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
@@ -2773,6 +2768,9 @@
       </c>
       <c r="AA36" s="4">
         <v>5.7353000000000001E-2</v>
+      </c>
+      <c r="AB36" s="4">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.25">
@@ -2802,6 +2800,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
       <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
@@ -2881,6 +2880,9 @@
       </c>
       <c r="AA38" s="4">
         <v>0.02</v>
+      </c>
+      <c r="AB38" s="4">
+        <v>9.5499999999999995E-3</v>
       </c>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.25">
@@ -2958,6 +2960,9 @@
         <v>0.1</v>
       </c>
       <c r="AA39" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB39" s="4">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>